<commit_message>
Updating with manually curated data.
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2013 Data/BogUpper5-R10.xlsx
+++ b/Data/phenotypic data/RawData/2013 Data/BogUpper5-R10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14370"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="25440" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3675" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3674" uniqueCount="218">
   <si>
     <t>Date measured:</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>1.940*</t>
-  </si>
-  <si>
-    <t>12.30*</t>
   </si>
   <si>
     <t>Row/Col: R10C6</t>
@@ -591,9 +588,6 @@
   </si>
   <si>
     <t>5.3/4.5</t>
-  </si>
-  <si>
-    <t>LB</t>
   </si>
   <si>
     <t>m</t>
@@ -986,11 +980,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1294,13 +1288,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:Y581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A545" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W583" sqref="W583"/>
+    <sheetView tabSelected="1" topLeftCell="A564" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V572" sqref="V572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" customWidth="1"/>
+    <col min="21" max="21" width="5.28515625" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" customWidth="1"/>
     <col min="23" max="23" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1351,10 +1366,10 @@
       <c r="L4" s="13"/>
       <c r="M4" s="12"/>
       <c r="N4" s="14"/>
-      <c r="O4" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="49"/>
+      <c r="O4" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="48"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="11"/>
       <c r="S4" s="16"/>
@@ -1375,11 +1390,11 @@
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="18"/>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
       <c r="N5" s="20" t="s">
         <v>5</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>43</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -3080,10 +3095,10 @@
       <c r="L33" s="13"/>
       <c r="M33" s="12"/>
       <c r="N33" s="14"/>
-      <c r="O33" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P33" s="49"/>
+      <c r="O33" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P33" s="48"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="11"/>
       <c r="S33" s="16"/>
@@ -3104,11 +3119,11 @@
       </c>
       <c r="I34" s="11"/>
       <c r="J34" s="18"/>
-      <c r="K34" s="48" t="s">
+      <c r="K34" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
       <c r="N34" s="20" t="s">
         <v>5</v>
       </c>
@@ -3318,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K38" s="34">
         <v>13.6</v>
@@ -3965,8 +3980,8 @@
       <c r="L47" s="34">
         <v>13.7</v>
       </c>
-      <c r="M47" s="34" t="s">
-        <v>71</v>
+      <c r="M47" s="34">
+        <v>1.23</v>
       </c>
       <c r="N47" s="35">
         <v>3</v>
@@ -4809,10 +4824,10 @@
       <c r="L62" s="13"/>
       <c r="M62" s="12"/>
       <c r="N62" s="14"/>
-      <c r="O62" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P62" s="49"/>
+      <c r="O62" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P62" s="48"/>
       <c r="Q62" s="15"/>
       <c r="R62" s="11"/>
       <c r="S62" s="16"/>
@@ -4833,11 +4848,11 @@
       </c>
       <c r="I63" s="11"/>
       <c r="J63" s="18"/>
-      <c r="K63" s="48" t="s">
+      <c r="K63" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L63" s="48"/>
-      <c r="M63" s="48"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="49"/>
       <c r="N63" s="20" t="s">
         <v>5</v>
       </c>
@@ -4994,7 +5009,7 @@
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" s="29"/>
       <c r="C66" s="29"/>
@@ -5053,7 +5068,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="L67" s="34">
-        <v>17.2</v>
+        <v>12.2</v>
       </c>
       <c r="M67" s="34">
         <v>0.95</v>
@@ -5071,7 +5086,7 @@
         <v>54</v>
       </c>
       <c r="R67" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S67" s="34">
         <v>2</v>
@@ -5109,7 +5124,7 @@
         <v>0</v>
       </c>
       <c r="G68" s="22">
-        <v>2.04</v>
+        <v>5.04</v>
       </c>
       <c r="H68" s="22">
         <v>5.53</v>
@@ -5142,7 +5157,7 @@
         <v>54</v>
       </c>
       <c r="R68" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S68" s="34">
         <v>1</v>
@@ -5213,13 +5228,13 @@
         <v>53</v>
       </c>
       <c r="R69" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S69" s="34">
         <v>1</v>
       </c>
       <c r="T69" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U69" s="34">
         <v>14</v>
@@ -5284,7 +5299,7 @@
         <v>53</v>
       </c>
       <c r="R70" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S70" s="34">
         <v>1</v>
@@ -5355,7 +5370,7 @@
         <v>53</v>
       </c>
       <c r="R71" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S71" s="34">
         <v>1</v>
@@ -5426,7 +5441,7 @@
         <v>53</v>
       </c>
       <c r="R72" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S72" s="34">
         <v>2</v>
@@ -5494,10 +5509,10 @@
         <v>52</v>
       </c>
       <c r="Q73" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="R73" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="R73" s="22" t="s">
-        <v>112</v>
       </c>
       <c r="S73" s="34">
         <v>2</v>
@@ -5754,7 +5769,7 @@
     </row>
     <row r="78" spans="1:23">
       <c r="A78" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -5824,14 +5839,14 @@
       <c r="O79" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P79" s="37" t="s">
-        <v>58</v>
+      <c r="P79" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="Q79" s="22" t="s">
         <v>54</v>
       </c>
       <c r="R79" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S79" s="34">
         <v>2</v>
@@ -5895,8 +5910,8 @@
       <c r="O80" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P80" s="37" t="s">
-        <v>58</v>
+      <c r="P80" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="Q80" s="22" t="s">
         <v>53</v>
@@ -5966,8 +5981,8 @@
       <c r="O81" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="P81" s="37" t="s">
-        <v>50</v>
+      <c r="P81" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="Q81" s="22" t="s">
         <v>53</v>
@@ -6037,8 +6052,8 @@
       <c r="O82" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P82" s="37" t="s">
-        <v>58</v>
+      <c r="P82" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="Q82" s="22" t="s">
         <v>53</v>
@@ -6108,8 +6123,8 @@
       <c r="O83" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P83" s="37" t="s">
-        <v>58</v>
+      <c r="P83" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="Q83" s="22" t="s">
         <v>53</v>
@@ -6179,8 +6194,8 @@
       <c r="O84" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P84" s="37" t="s">
-        <v>58</v>
+      <c r="P84" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="Q84" s="22" t="s">
         <v>54</v>
@@ -6250,7 +6265,7 @@
       <c r="O85" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="P85" s="37" t="s">
+      <c r="P85" s="15" t="s">
         <v>51</v>
       </c>
       <c r="Q85" s="22" t="s">
@@ -6321,8 +6336,8 @@
       <c r="O86" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P86" s="37" t="s">
-        <v>58</v>
+      <c r="P86" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="Q86" s="22" t="s">
         <v>53</v>
@@ -6392,14 +6407,14 @@
       <c r="O87" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P87" s="37" t="s">
-        <v>58</v>
+      <c r="P87" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="Q87" s="22" t="s">
         <v>54</v>
       </c>
       <c r="R87" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S87" s="34">
         <v>2</v>
@@ -6422,49 +6437,49 @@
         <v>10</v>
       </c>
       <c r="B88" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="43" t="s">
+      <c r="D88" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D88" s="43" t="s">
+      <c r="F88" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="E88" s="43" t="s">
+      <c r="G88" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="F88" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="G88" s="43" t="s">
+      <c r="H88" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="H88" s="43" t="s">
+      <c r="I88" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="J88" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="K88" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="I88" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="J88" s="47" t="s">
-        <v>214</v>
-      </c>
-      <c r="K88" s="44" t="s">
+      <c r="L88" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="L88" s="44" t="s">
+      <c r="M88" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="M88" s="44" t="s">
+      <c r="N88" s="44" t="s">
         <v>109</v>
-      </c>
-      <c r="N88" s="44" t="s">
-        <v>110</v>
       </c>
       <c r="O88" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="P88" s="44" t="s">
-        <v>51</v>
+      <c r="P88" s="47" t="s">
+        <v>64</v>
       </c>
       <c r="Q88" s="43" t="s">
         <v>54</v>
@@ -6473,19 +6488,19 @@
         <v>54</v>
       </c>
       <c r="S88" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T88" s="44" t="s">
         <v>58</v>
       </c>
       <c r="U88" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="V88" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="V88" s="43" t="s">
-        <v>117</v>
-      </c>
       <c r="W88" s="45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="X88" s="45"/>
       <c r="Y88" s="45"/>
@@ -6537,10 +6552,10 @@
       <c r="L91" s="13"/>
       <c r="M91" s="12"/>
       <c r="N91" s="14"/>
-      <c r="O91" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P91" s="49"/>
+      <c r="O91" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P91" s="48"/>
       <c r="Q91" s="15"/>
       <c r="R91" s="11"/>
       <c r="S91" s="16"/>
@@ -6561,11 +6576,11 @@
       </c>
       <c r="I92" s="11"/>
       <c r="J92" s="18"/>
-      <c r="K92" s="48" t="s">
+      <c r="K92" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L92" s="48"/>
-      <c r="M92" s="48"/>
+      <c r="L92" s="49"/>
+      <c r="M92" s="49"/>
       <c r="N92" s="20" t="s">
         <v>5</v>
       </c>
@@ -6722,7 +6737,7 @@
     </row>
     <row r="95" spans="1:25">
       <c r="A95" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B95" s="29"/>
       <c r="C95" s="29"/>
@@ -6766,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="G96" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H96" s="22">
         <v>3.1</v>
@@ -6802,7 +6817,7 @@
         <v>56</v>
       </c>
       <c r="S96" s="34">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="T96" s="34" t="s">
         <v>58</v>
@@ -6873,7 +6888,7 @@
         <v>54</v>
       </c>
       <c r="S97" s="34">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="T97" s="34" t="s">
         <v>58</v>
@@ -6944,7 +6959,7 @@
         <v>54</v>
       </c>
       <c r="S98" s="34">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="T98" s="34" t="s">
         <v>58</v>
@@ -7015,7 +7030,7 @@
         <v>56</v>
       </c>
       <c r="S99" s="34">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="T99" s="34" t="s">
         <v>57</v>
@@ -7086,7 +7101,7 @@
         <v>56</v>
       </c>
       <c r="S100" s="34">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="T100" s="34" t="s">
         <v>57</v>
@@ -7157,7 +7172,7 @@
         <v>56</v>
       </c>
       <c r="S101" s="34">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="T101" s="34" t="s">
         <v>57</v>
@@ -7228,7 +7243,7 @@
         <v>56</v>
       </c>
       <c r="S102" s="34">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="T102" s="34" t="s">
         <v>57</v>
@@ -7299,7 +7314,7 @@
         <v>56</v>
       </c>
       <c r="S103" s="34">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="T103" s="34" t="s">
         <v>57</v>
@@ -7370,7 +7385,7 @@
         <v>54</v>
       </c>
       <c r="S104" s="34">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="T104" s="34" t="s">
         <v>58</v>
@@ -7441,10 +7456,10 @@
         <v>56</v>
       </c>
       <c r="S105" s="34">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="T105" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U105" s="34">
         <v>27</v>
@@ -7482,7 +7497,7 @@
     </row>
     <row r="107" spans="1:23">
       <c r="A107" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
@@ -7562,7 +7577,7 @@
         <v>53</v>
       </c>
       <c r="S108" s="34">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="T108" s="34" t="s">
         <v>57</v>
@@ -7633,7 +7648,7 @@
         <v>54</v>
       </c>
       <c r="S109" s="34">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="T109" s="34" t="s">
         <v>57</v>
@@ -7668,7 +7683,7 @@
         <v>2</v>
       </c>
       <c r="G110" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H110" s="22">
         <v>4.2</v>
@@ -7686,7 +7701,7 @@
         <v>17.3</v>
       </c>
       <c r="M110" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N110" s="35">
         <v>2.9</v>
@@ -7704,7 +7719,7 @@
         <v>54</v>
       </c>
       <c r="S110" s="34">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="T110" s="34" t="s">
         <v>58</v>
@@ -7775,7 +7790,7 @@
         <v>53</v>
       </c>
       <c r="S111" s="34">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="T111" s="34" t="s">
         <v>57</v>
@@ -7846,7 +7861,7 @@
         <v>53</v>
       </c>
       <c r="S112" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T112" s="34" t="s">
         <v>57</v>
@@ -7910,14 +7925,14 @@
       <c r="P113" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="Q113" s="22" t="s">
-        <v>53</v>
+      <c r="Q113" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="R113" s="22" t="s">
         <v>53</v>
       </c>
       <c r="S113" s="34">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="T113" s="34" t="s">
         <v>57</v>
@@ -7952,7 +7967,7 @@
         <v>0</v>
       </c>
       <c r="G114" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H114" s="22">
         <v>2.2000000000000002</v>
@@ -7988,7 +8003,7 @@
         <v>54</v>
       </c>
       <c r="S114" s="34">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="T114" s="34" t="s">
         <v>58</v>
@@ -8059,7 +8074,7 @@
         <v>53</v>
       </c>
       <c r="S115" s="34">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="T115" s="34" t="s">
         <v>57</v>
@@ -8130,7 +8145,7 @@
         <v>54</v>
       </c>
       <c r="S116" s="34">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="T116" s="34" t="s">
         <v>58</v>
@@ -8201,7 +8216,7 @@
         <v>53</v>
       </c>
       <c r="S117" s="34">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="T117" s="34" t="s">
         <v>57</v>
@@ -8263,10 +8278,10 @@
       <c r="L120" s="13"/>
       <c r="M120" s="12"/>
       <c r="N120" s="14"/>
-      <c r="O120" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P120" s="49"/>
+      <c r="O120" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P120" s="48"/>
       <c r="Q120" s="15"/>
       <c r="R120" s="11"/>
       <c r="S120" s="16"/>
@@ -8287,11 +8302,11 @@
       </c>
       <c r="I121" s="11"/>
       <c r="J121" s="18"/>
-      <c r="K121" s="48" t="s">
+      <c r="K121" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L121" s="48"/>
-      <c r="M121" s="48"/>
+      <c r="L121" s="49"/>
+      <c r="M121" s="49"/>
       <c r="N121" s="20" t="s">
         <v>5</v>
       </c>
@@ -8448,7 +8463,7 @@
     </row>
     <row r="124" spans="1:23">
       <c r="A124" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B124" s="29"/>
       <c r="C124" s="29"/>
@@ -8563,7 +8578,7 @@
         <v>2</v>
       </c>
       <c r="G126" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H126" s="22">
         <v>7</v>
@@ -8705,7 +8720,7 @@
         <v>0</v>
       </c>
       <c r="G128" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H128" s="22">
         <v>2.1</v>
@@ -8723,7 +8738,7 @@
         <v>9.6</v>
       </c>
       <c r="M128" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N128" s="35">
         <v>2.4</v>
@@ -8806,7 +8821,7 @@
         <v>52</v>
       </c>
       <c r="Q129" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R129" s="22" t="s">
         <v>54</v>
@@ -8853,7 +8868,7 @@
         <v>1</v>
       </c>
       <c r="I130" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J130" s="34">
         <v>4.7E-2</v>
@@ -9060,7 +9075,7 @@
         <v>0</v>
       </c>
       <c r="G133" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H133" s="22">
         <v>4.5</v>
@@ -9078,7 +9093,7 @@
         <v>9</v>
       </c>
       <c r="M133" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N133" s="35">
         <v>2.6</v>
@@ -9116,7 +9131,7 @@
         <v>10</v>
       </c>
       <c r="B134" s="22">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C134" s="22">
         <v>1</v>
@@ -9131,7 +9146,7 @@
         <v>3</v>
       </c>
       <c r="G134" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H134" s="22">
         <v>2.7</v>
@@ -9149,7 +9164,7 @@
         <v>14.1</v>
       </c>
       <c r="M134" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N134" s="35">
         <v>3.1</v>
@@ -9164,13 +9179,13 @@
         <v>54</v>
       </c>
       <c r="R134" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S134" s="34">
         <v>1</v>
       </c>
       <c r="T134" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U134" s="34">
         <v>15</v>
@@ -9208,7 +9223,7 @@
     </row>
     <row r="136" spans="1:23">
       <c r="A136" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B136" s="12"/>
       <c r="C136" s="12"/>
@@ -9465,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="G140" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H140" s="22">
         <v>4.3</v>
@@ -9483,7 +9498,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="M140" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N140" s="35">
         <v>3.3</v>
@@ -9640,13 +9655,13 @@
         <v>53</v>
       </c>
       <c r="R142" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S142" s="34">
         <v>1</v>
       </c>
       <c r="T142" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U142" s="34">
         <v>29</v>
@@ -9811,7 +9826,7 @@
         <v>0</v>
       </c>
       <c r="D145" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E145" s="22">
         <v>1</v>
@@ -9989,10 +10004,10 @@
       <c r="L149" s="13"/>
       <c r="M149" s="12"/>
       <c r="N149" s="14"/>
-      <c r="O149" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P149" s="49"/>
+      <c r="O149" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P149" s="48"/>
       <c r="Q149" s="15"/>
       <c r="R149" s="11"/>
       <c r="S149" s="16"/>
@@ -10013,11 +10028,11 @@
       </c>
       <c r="I150" s="11"/>
       <c r="J150" s="18"/>
-      <c r="K150" s="48" t="s">
+      <c r="K150" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L150" s="48"/>
-      <c r="M150" s="48"/>
+      <c r="L150" s="49"/>
+      <c r="M150" s="49"/>
       <c r="N150" s="20" t="s">
         <v>5</v>
       </c>
@@ -10174,7 +10189,7 @@
     </row>
     <row r="153" spans="1:23">
       <c r="A153" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B153" s="29"/>
       <c r="C153" s="29"/>
@@ -10257,7 +10272,7 @@
         <v>1</v>
       </c>
       <c r="T154" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U154" s="34">
         <v>28</v>
@@ -10464,13 +10479,13 @@
         <v>53</v>
       </c>
       <c r="R157" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S157" s="34">
         <v>2</v>
       </c>
       <c r="T157" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U157" s="34">
         <v>10</v>
@@ -10612,7 +10627,7 @@
         <v>1</v>
       </c>
       <c r="T159" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U159" s="34">
         <v>20</v>
@@ -10825,7 +10840,7 @@
         <v>1</v>
       </c>
       <c r="T162" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U162" s="34">
         <v>15</v>
@@ -10934,7 +10949,7 @@
     </row>
     <row r="165" spans="1:23">
       <c r="A165" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
@@ -11034,43 +11049,43 @@
         <v>2</v>
       </c>
       <c r="B167" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C167" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D167" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="E167" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="E167" s="43" t="s">
-        <v>133</v>
-      </c>
       <c r="F167" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G167" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H167" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I167" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J167" s="47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K167" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L167" s="44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M167" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="N167" s="44" t="s">
         <v>143</v>
-      </c>
-      <c r="N167" s="44" t="s">
-        <v>144</v>
       </c>
       <c r="O167" s="44" t="s">
         <v>50</v>
@@ -11085,16 +11100,16 @@
         <v>54</v>
       </c>
       <c r="S167" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T167" s="44" t="s">
         <v>58</v>
       </c>
       <c r="U167" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V167" s="43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W167">
         <v>1</v>
@@ -11224,7 +11239,7 @@
         <v>54</v>
       </c>
       <c r="R169" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S169" s="34">
         <v>1</v>
@@ -11247,43 +11262,43 @@
         <v>5</v>
       </c>
       <c r="B170" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C170" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D170" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="C170" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D170" s="43" t="s">
+      <c r="E170" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="F170" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="E170" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="F170" s="43" t="s">
-        <v>131</v>
-      </c>
       <c r="G170" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H170" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I170" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J170" s="47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K170" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L170" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M170" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N170" s="44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O170" s="44" t="s">
         <v>50</v>
@@ -11298,16 +11313,16 @@
         <v>54</v>
       </c>
       <c r="S170" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T170" s="44" t="s">
         <v>58</v>
       </c>
       <c r="U170" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="V170" s="43" t="s">
         <v>147</v>
-      </c>
-      <c r="V170" s="43" t="s">
-        <v>148</v>
       </c>
       <c r="W170">
         <v>1</v>
@@ -11366,7 +11381,7 @@
         <v>54</v>
       </c>
       <c r="R171" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S171" s="34">
         <v>2</v>
@@ -11505,10 +11520,10 @@
         <v>64</v>
       </c>
       <c r="Q173" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R173" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S173" s="34">
         <v>1</v>
@@ -11715,10 +11730,10 @@
       <c r="L178" s="13"/>
       <c r="M178" s="12"/>
       <c r="N178" s="14"/>
-      <c r="O178" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P178" s="49"/>
+      <c r="O178" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P178" s="48"/>
       <c r="Q178" s="15"/>
       <c r="R178" s="11"/>
       <c r="S178" s="16"/>
@@ -11739,11 +11754,11 @@
       </c>
       <c r="I179" s="11"/>
       <c r="J179" s="18"/>
-      <c r="K179" s="48" t="s">
+      <c r="K179" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L179" s="48"/>
-      <c r="M179" s="48"/>
+      <c r="L179" s="49"/>
+      <c r="M179" s="49"/>
       <c r="N179" s="20" t="s">
         <v>5</v>
       </c>
@@ -11900,7 +11915,7 @@
     </row>
     <row r="182" spans="1:23">
       <c r="A182" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B182" s="29"/>
       <c r="C182" s="29"/>
@@ -11977,7 +11992,7 @@
         <v>54</v>
       </c>
       <c r="R183" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S183" s="34">
         <v>1</v>
@@ -12190,7 +12205,7 @@
         <v>54</v>
       </c>
       <c r="R186" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S186" s="34">
         <v>2</v>
@@ -12261,7 +12276,7 @@
         <v>54</v>
       </c>
       <c r="R187" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S187" s="34">
         <v>2</v>
@@ -12332,7 +12347,7 @@
         <v>54</v>
       </c>
       <c r="R188" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S188" s="34">
         <v>2</v>
@@ -12403,7 +12418,7 @@
         <v>54</v>
       </c>
       <c r="R189" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S189" s="34">
         <v>1</v>
@@ -12474,13 +12489,13 @@
         <v>54</v>
       </c>
       <c r="R190" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S190" s="34">
         <v>2</v>
       </c>
       <c r="T190" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U190" s="34">
         <v>23</v>
@@ -12660,7 +12675,7 @@
     </row>
     <row r="194" spans="1:23">
       <c r="A194" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B194" s="12"/>
       <c r="C194" s="12"/>
@@ -12808,7 +12823,7 @@
         <v>54</v>
       </c>
       <c r="R196" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S196" s="34">
         <v>2</v>
@@ -12876,7 +12891,7 @@
         <v>51</v>
       </c>
       <c r="Q197" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R197" s="22" t="s">
         <v>53</v>
@@ -12885,7 +12900,7 @@
         <v>2</v>
       </c>
       <c r="T197" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U197" s="34">
         <v>21</v>
@@ -12947,7 +12962,7 @@
         <v>51</v>
       </c>
       <c r="Q198" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R198" s="22" t="s">
         <v>53</v>
@@ -13089,7 +13104,7 @@
         <v>52</v>
       </c>
       <c r="Q200" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R200" s="22" t="s">
         <v>53</v>
@@ -13160,7 +13175,7 @@
         <v>51</v>
       </c>
       <c r="Q201" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R201" s="22" t="s">
         <v>54</v>
@@ -13302,7 +13317,7 @@
         <v>52</v>
       </c>
       <c r="Q203" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R203" s="22" t="s">
         <v>54</v>
@@ -13373,7 +13388,7 @@
         <v>51</v>
       </c>
       <c r="Q204" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R204" s="22" t="s">
         <v>53</v>
@@ -13396,7 +13411,7 @@
     </row>
     <row r="206" spans="1:23" ht="15.75">
       <c r="A206" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -13441,10 +13456,10 @@
       <c r="L207" s="13"/>
       <c r="M207" s="12"/>
       <c r="N207" s="14"/>
-      <c r="O207" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P207" s="49"/>
+      <c r="O207" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P207" s="48"/>
       <c r="Q207" s="15"/>
       <c r="R207" s="11"/>
       <c r="S207" s="16"/>
@@ -13465,11 +13480,11 @@
       </c>
       <c r="I208" s="11"/>
       <c r="J208" s="18"/>
-      <c r="K208" s="48" t="s">
+      <c r="K208" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L208" s="48"/>
-      <c r="M208" s="48"/>
+      <c r="L208" s="49"/>
+      <c r="M208" s="49"/>
       <c r="N208" s="20" t="s">
         <v>5</v>
       </c>
@@ -13626,7 +13641,7 @@
     </row>
     <row r="211" spans="1:23">
       <c r="A211" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B211" s="29"/>
       <c r="C211" s="29"/>
@@ -13774,7 +13789,7 @@
         <v>54</v>
       </c>
       <c r="R213" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S213" s="34">
         <v>2</v>
@@ -13842,10 +13857,10 @@
         <v>64</v>
       </c>
       <c r="Q214" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R214" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S214" s="34">
         <v>2</v>
@@ -13913,10 +13928,10 @@
         <v>64</v>
       </c>
       <c r="Q215" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R215" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S215" s="34">
         <v>1</v>
@@ -13987,7 +14002,7 @@
         <v>54</v>
       </c>
       <c r="R216" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S216" s="34">
         <v>1</v>
@@ -14055,7 +14070,7 @@
         <v>64</v>
       </c>
       <c r="Q217" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R217" s="22" t="s">
         <v>54</v>
@@ -14126,10 +14141,10 @@
         <v>64</v>
       </c>
       <c r="Q218" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R218" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S218" s="34">
         <v>1</v>
@@ -14250,7 +14265,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="K220" s="34">
-        <v>20</v>
+        <v>20.6</v>
       </c>
       <c r="L220" s="34">
         <v>15.1</v>
@@ -14271,7 +14286,7 @@
         <v>54</v>
       </c>
       <c r="R220" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S220" s="34">
         <v>1</v>
@@ -14386,7 +14401,7 @@
     </row>
     <row r="223" spans="1:23">
       <c r="A223" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
@@ -14436,7 +14451,7 @@
         <v>7.72</v>
       </c>
       <c r="I224" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J224" s="34">
         <v>0.222</v>
@@ -14475,7 +14490,7 @@
         <v>27</v>
       </c>
       <c r="V224" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W224">
         <v>1</v>
@@ -14605,13 +14620,13 @@
         <v>53</v>
       </c>
       <c r="R226" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S226" s="34">
         <v>2</v>
       </c>
       <c r="T226" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U226" s="34">
         <v>19</v>
@@ -14744,7 +14759,7 @@
         <v>51</v>
       </c>
       <c r="Q228" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R228" s="22" t="s">
         <v>54</v>
@@ -14753,7 +14768,7 @@
         <v>2</v>
       </c>
       <c r="T228" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U228" s="34">
         <v>21</v>
@@ -14889,13 +14904,13 @@
         <v>53</v>
       </c>
       <c r="R230" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S230" s="34">
         <v>1</v>
       </c>
       <c r="T230" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U230" s="34">
         <v>7</v>
@@ -14960,7 +14975,7 @@
         <v>54</v>
       </c>
       <c r="R231" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S231" s="34">
         <v>1</v>
@@ -15102,7 +15117,7 @@
         <v>54</v>
       </c>
       <c r="R233" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S233" s="34">
         <v>3</v>
@@ -15167,10 +15182,10 @@
       <c r="L236" s="13"/>
       <c r="M236" s="12"/>
       <c r="N236" s="14"/>
-      <c r="O236" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P236" s="49"/>
+      <c r="O236" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P236" s="48"/>
       <c r="Q236" s="15"/>
       <c r="R236" s="11"/>
       <c r="S236" s="16"/>
@@ -15191,11 +15206,11 @@
       </c>
       <c r="I237" s="11"/>
       <c r="J237" s="18"/>
-      <c r="K237" s="48" t="s">
+      <c r="K237" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L237" s="48"/>
-      <c r="M237" s="48"/>
+      <c r="L237" s="49"/>
+      <c r="M237" s="49"/>
       <c r="N237" s="20" t="s">
         <v>5</v>
       </c>
@@ -15352,7 +15367,7 @@
     </row>
     <row r="240" spans="1:23">
       <c r="A240" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B240" s="29"/>
       <c r="C240" s="29"/>
@@ -15396,7 +15411,7 @@
         <v>3</v>
       </c>
       <c r="G241" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H241" s="22">
         <v>3.6</v>
@@ -15429,7 +15444,7 @@
         <v>53</v>
       </c>
       <c r="R241" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S241" s="34">
         <v>2</v>
@@ -15713,7 +15728,7 @@
         <v>54</v>
       </c>
       <c r="R245" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S245" s="34">
         <v>1</v>
@@ -15784,7 +15799,7 @@
         <v>53</v>
       </c>
       <c r="R246" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S246" s="34">
         <v>1</v>
@@ -15893,7 +15908,7 @@
         <v>0</v>
       </c>
       <c r="G248" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H248" s="22">
         <v>3.4</v>
@@ -16112,7 +16127,7 @@
     </row>
     <row r="252" spans="1:23">
       <c r="A252" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B252" s="12"/>
       <c r="C252" s="12"/>
@@ -16724,7 +16739,7 @@
         <v>1</v>
       </c>
       <c r="G261" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H261" s="22">
         <v>3.4</v>
@@ -16848,7 +16863,7 @@
     </row>
     <row r="264" spans="1:23" ht="15.75">
       <c r="A264" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
@@ -16893,10 +16908,10 @@
       <c r="L265" s="13"/>
       <c r="M265" s="12"/>
       <c r="N265" s="14"/>
-      <c r="O265" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P265" s="49"/>
+      <c r="O265" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P265" s="48"/>
       <c r="Q265" s="15"/>
       <c r="R265" s="11"/>
       <c r="S265" s="16"/>
@@ -16917,11 +16932,11 @@
       </c>
       <c r="I266" s="11"/>
       <c r="J266" s="18"/>
-      <c r="K266" s="48" t="s">
+      <c r="K266" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L266" s="48"/>
-      <c r="M266" s="48"/>
+      <c r="L266" s="49"/>
+      <c r="M266" s="49"/>
       <c r="N266" s="20" t="s">
         <v>5</v>
       </c>
@@ -17078,7 +17093,7 @@
     </row>
     <row r="269" spans="1:23">
       <c r="A269" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B269" s="29"/>
       <c r="C269" s="29"/>
@@ -17800,7 +17815,7 @@
         <v>1</v>
       </c>
       <c r="T279" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U279" s="34">
         <v>26</v>
@@ -17838,7 +17853,7 @@
     </row>
     <row r="281" spans="1:23">
       <c r="A281" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B281" s="12"/>
       <c r="C281" s="12"/>
@@ -17882,7 +17897,7 @@
         <v>1</v>
       </c>
       <c r="G282" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H282" s="22">
         <v>4.3</v>
@@ -17900,7 +17915,7 @@
         <v>16.8</v>
       </c>
       <c r="M282" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N282" s="35">
         <v>2.4</v>
@@ -18308,7 +18323,7 @@
         <v>0</v>
       </c>
       <c r="G288" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H288" s="22">
         <v>5.2</v>
@@ -18379,7 +18394,7 @@
         <v>0</v>
       </c>
       <c r="G289" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H289" s="22">
         <v>4.4000000000000004</v>
@@ -18412,13 +18427,13 @@
         <v>53</v>
       </c>
       <c r="R289" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S289" s="34">
         <v>1</v>
       </c>
       <c r="T289" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U289" s="34">
         <v>8</v>
@@ -18450,7 +18465,7 @@
         <v>1</v>
       </c>
       <c r="G290" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H290" s="22">
         <v>4.0999999999999996</v>
@@ -18483,7 +18498,7 @@
         <v>54</v>
       </c>
       <c r="R290" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S290" s="34">
         <v>1</v>
@@ -18554,7 +18569,7 @@
         <v>54</v>
       </c>
       <c r="R291" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S291" s="34">
         <v>2</v>
@@ -18574,7 +18589,7 @@
     </row>
     <row r="293" spans="1:23" ht="15.75">
       <c r="A293" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
@@ -18619,10 +18634,10 @@
       <c r="L294" s="13"/>
       <c r="M294" s="12"/>
       <c r="N294" s="14"/>
-      <c r="O294" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P294" s="49"/>
+      <c r="O294" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P294" s="48"/>
       <c r="Q294" s="15"/>
       <c r="R294" s="11"/>
       <c r="S294" s="16"/>
@@ -18643,11 +18658,11 @@
       </c>
       <c r="I295" s="11"/>
       <c r="J295" s="18"/>
-      <c r="K295" s="48" t="s">
+      <c r="K295" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L295" s="48"/>
-      <c r="M295" s="48"/>
+      <c r="L295" s="49"/>
+      <c r="M295" s="49"/>
       <c r="N295" s="20" t="s">
         <v>5</v>
       </c>
@@ -18804,7 +18819,7 @@
     </row>
     <row r="298" spans="1:23">
       <c r="A298" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B298" s="29"/>
       <c r="C298" s="29"/>
@@ -18848,7 +18863,7 @@
         <v>0</v>
       </c>
       <c r="G299" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H299" s="22">
         <v>5.0999999999999996</v>
@@ -18866,7 +18881,7 @@
         <v>18</v>
       </c>
       <c r="M299" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N299" s="35">
         <v>2.5</v>
@@ -19203,7 +19218,7 @@
         <v>0</v>
       </c>
       <c r="G304" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H304" s="22">
         <v>8.4</v>
@@ -19487,7 +19502,7 @@
         <v>1</v>
       </c>
       <c r="G308" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H308" s="22">
         <v>3.3</v>
@@ -19564,7 +19579,7 @@
     </row>
     <row r="310" spans="1:23">
       <c r="A310" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B310" s="12"/>
       <c r="C310" s="12"/>
@@ -19969,7 +19984,7 @@
         <v>2.9</v>
       </c>
       <c r="I316" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J316" s="34">
         <v>0.14499999999999999</v>
@@ -20034,7 +20049,7 @@
         <v>0</v>
       </c>
       <c r="G317" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H317" s="22">
         <v>3.5</v>
@@ -20300,7 +20315,7 @@
     </row>
     <row r="322" spans="1:23" ht="15.75">
       <c r="A322" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
@@ -20345,10 +20360,10 @@
       <c r="L323" s="13"/>
       <c r="M323" s="12"/>
       <c r="N323" s="14"/>
-      <c r="O323" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P323" s="49"/>
+      <c r="O323" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P323" s="48"/>
       <c r="Q323" s="15"/>
       <c r="R323" s="11"/>
       <c r="S323" s="16"/>
@@ -20369,11 +20384,11 @@
       </c>
       <c r="I324" s="11"/>
       <c r="J324" s="18"/>
-      <c r="K324" s="48" t="s">
+      <c r="K324" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L324" s="48"/>
-      <c r="M324" s="48"/>
+      <c r="L324" s="49"/>
+      <c r="M324" s="49"/>
       <c r="N324" s="20" t="s">
         <v>5</v>
       </c>
@@ -20530,7 +20545,7 @@
     </row>
     <row r="327" spans="1:23">
       <c r="A327" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B327" s="29"/>
       <c r="C327" s="29"/>
@@ -20574,13 +20589,13 @@
         <v>2</v>
       </c>
       <c r="G328" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H328" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I328" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J328" s="34">
         <v>0.15</v>
@@ -20592,7 +20607,7 @@
         <v>16.5</v>
       </c>
       <c r="M328" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N328" s="35">
         <v>2.7</v>
@@ -20716,10 +20731,10 @@
         <v>1</v>
       </c>
       <c r="G330" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H330" s="22">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="I330" s="22">
         <v>0.6</v>
@@ -20734,7 +20749,7 @@
         <v>17.5</v>
       </c>
       <c r="M330" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N330" s="35">
         <v>2.9</v>
@@ -20790,7 +20805,7 @@
         <v>6.6070000000000002</v>
       </c>
       <c r="H331" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I331" s="22">
         <v>0</v>
@@ -21219,7 +21234,7 @@
         <v>4.5</v>
       </c>
       <c r="I337" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J337" s="34">
         <v>0.151</v>
@@ -21290,7 +21305,7 @@
     </row>
     <row r="339" spans="1:23">
       <c r="A339" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B339" s="12"/>
       <c r="C339" s="12"/>
@@ -21438,7 +21453,7 @@
         <v>54</v>
       </c>
       <c r="R341" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S341" s="34">
         <v>1</v>
@@ -21580,7 +21595,7 @@
         <v>54</v>
       </c>
       <c r="R343" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S343" s="34">
         <v>3</v>
@@ -21651,7 +21666,7 @@
         <v>53</v>
       </c>
       <c r="R344" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S344" s="34">
         <v>1</v>
@@ -21722,7 +21737,7 @@
         <v>54</v>
       </c>
       <c r="R345" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S345" s="34">
         <v>2</v>
@@ -21864,7 +21879,7 @@
         <v>54</v>
       </c>
       <c r="R347" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S347" s="34">
         <v>3</v>
@@ -22006,7 +22021,7 @@
         <v>54</v>
       </c>
       <c r="R349" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S349" s="34">
         <v>1</v>
@@ -22026,7 +22041,7 @@
     </row>
     <row r="351" spans="1:23" ht="15.75">
       <c r="A351" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
@@ -22071,10 +22086,10 @@
       <c r="L352" s="13"/>
       <c r="M352" s="12"/>
       <c r="N352" s="14"/>
-      <c r="O352" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P352" s="49"/>
+      <c r="O352" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P352" s="48"/>
       <c r="Q352" s="15"/>
       <c r="R352" s="11"/>
       <c r="S352" s="16"/>
@@ -22095,11 +22110,11 @@
       </c>
       <c r="I353" s="11"/>
       <c r="J353" s="18"/>
-      <c r="K353" s="48" t="s">
+      <c r="K353" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L353" s="48"/>
-      <c r="M353" s="48"/>
+      <c r="L353" s="49"/>
+      <c r="M353" s="49"/>
       <c r="N353" s="20" t="s">
         <v>5</v>
       </c>
@@ -22256,7 +22271,7 @@
     </row>
     <row r="356" spans="1:23">
       <c r="A356" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B356" s="29"/>
       <c r="C356" s="29"/>
@@ -22285,19 +22300,19 @@
         <v>1</v>
       </c>
       <c r="B357" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C357" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C357" s="22" t="s">
+      <c r="D357" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="D357" s="22" t="s">
+      <c r="E357" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F357" s="46" t="s">
         <v>179</v>
-      </c>
-      <c r="E357" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="F357" s="46" t="s">
-        <v>180</v>
       </c>
       <c r="G357" s="22">
         <v>5.3810000000000002</v>
@@ -22602,7 +22617,7 @@
         <v>16.2</v>
       </c>
       <c r="M361" s="34">
-        <v>2034</v>
+        <v>2.0339999999999998</v>
       </c>
       <c r="N361" s="35">
         <v>3.3</v>
@@ -23016,7 +23031,7 @@
     </row>
     <row r="368" spans="1:23">
       <c r="A368" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B368" s="12"/>
       <c r="C368" s="12"/>
@@ -23075,7 +23090,7 @@
         <v>22.1</v>
       </c>
       <c r="L369" s="34">
-        <v>12.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="M369" s="34">
         <v>2.7130000000000001</v>
@@ -23146,7 +23161,7 @@
         <v>18.8</v>
       </c>
       <c r="L370" s="34">
-        <v>16.7</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="M370" s="34">
         <v>2.08</v>
@@ -23217,7 +23232,7 @@
         <v>18.7</v>
       </c>
       <c r="L371" s="34">
-        <v>16.7</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="M371" s="34">
         <v>2.1179999999999999</v>
@@ -23755,7 +23770,7 @@
     </row>
     <row r="380" spans="1:23" ht="15.75">
       <c r="A380" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
@@ -23800,10 +23815,10 @@
       <c r="L381" s="13"/>
       <c r="M381" s="12"/>
       <c r="N381" s="14"/>
-      <c r="O381" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P381" s="49"/>
+      <c r="O381" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P381" s="48"/>
       <c r="Q381" s="15"/>
       <c r="R381" s="11"/>
       <c r="S381" s="16"/>
@@ -23824,11 +23839,11 @@
       </c>
       <c r="I382" s="11"/>
       <c r="J382" s="18"/>
-      <c r="K382" s="48" t="s">
+      <c r="K382" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L382" s="48"/>
-      <c r="M382" s="48"/>
+      <c r="L382" s="49"/>
+      <c r="M382" s="49"/>
       <c r="N382" s="20" t="s">
         <v>5</v>
       </c>
@@ -23985,7 +24000,7 @@
     </row>
     <row r="385" spans="1:23">
       <c r="A385" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B385" s="29"/>
       <c r="C385" s="29"/>
@@ -24106,7 +24121,7 @@
         <v>3.7</v>
       </c>
       <c r="I387" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J387" s="34">
         <v>0.26200000000000001</v>
@@ -24174,7 +24189,7 @@
         <v>3.0169999999999999</v>
       </c>
       <c r="H388" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I388" s="22">
         <v>0</v>
@@ -24245,7 +24260,7 @@
         <v>6.6769999999999996</v>
       </c>
       <c r="H389" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I389" s="22">
         <v>0</v>
@@ -24351,8 +24366,8 @@
       <c r="S390" s="34">
         <v>1</v>
       </c>
-      <c r="T390" s="34" t="s">
-        <v>188</v>
+      <c r="T390" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="U390" s="34">
         <v>19</v>
@@ -24529,7 +24544,7 @@
         <v>5.5410000000000004</v>
       </c>
       <c r="H393" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I393" s="22">
         <v>0</v>
@@ -24671,7 +24686,7 @@
         <v>6.8239999999999998</v>
       </c>
       <c r="H395" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I395" s="22">
         <v>0</v>
@@ -24745,7 +24760,7 @@
     </row>
     <row r="397" spans="1:23">
       <c r="A397" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B397" s="12"/>
       <c r="C397" s="12"/>
@@ -24964,7 +24979,7 @@
         <v>54</v>
       </c>
       <c r="R400" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S400" s="34">
         <v>1</v>
@@ -25076,7 +25091,7 @@
         <v>2.3490000000000002</v>
       </c>
       <c r="H402" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I402" s="22">
         <v>0</v>
@@ -25165,7 +25180,7 @@
         <v>1.6</v>
       </c>
       <c r="N403" s="35">
-        <v>26</v>
+        <v>2.6</v>
       </c>
       <c r="O403" s="37" t="s">
         <v>51</v>
@@ -25289,7 +25304,7 @@
         <v>3.637</v>
       </c>
       <c r="H405" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I405" s="22">
         <v>0</v>
@@ -25390,7 +25405,7 @@
         <v>53</v>
       </c>
       <c r="R406" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S406" s="34">
         <v>2</v>
@@ -25481,7 +25496,7 @@
     </row>
     <row r="409" spans="1:23" ht="15.75">
       <c r="A409" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
@@ -25526,10 +25541,10 @@
       <c r="L410" s="13"/>
       <c r="M410" s="12"/>
       <c r="N410" s="14"/>
-      <c r="O410" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P410" s="49"/>
+      <c r="O410" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P410" s="48"/>
       <c r="Q410" s="15"/>
       <c r="R410" s="11"/>
       <c r="S410" s="16"/>
@@ -25550,11 +25565,11 @@
       </c>
       <c r="I411" s="11"/>
       <c r="J411" s="18"/>
-      <c r="K411" s="48" t="s">
+      <c r="K411" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L411" s="48"/>
-      <c r="M411" s="48"/>
+      <c r="L411" s="49"/>
+      <c r="M411" s="49"/>
       <c r="N411" s="20" t="s">
         <v>5</v>
       </c>
@@ -25711,7 +25726,7 @@
     </row>
     <row r="414" spans="1:23">
       <c r="A414" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B414" s="29"/>
       <c r="C414" s="29"/>
@@ -25779,13 +25794,13 @@
         <v>3.2</v>
       </c>
       <c r="O415" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P415" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Q415" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R415" s="22" t="s">
         <v>54</v>
@@ -25850,7 +25865,7 @@
         <v>3</v>
       </c>
       <c r="O416" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P416" s="37" t="s">
         <v>64</v>
@@ -25921,16 +25936,16 @@
         <v>2.8</v>
       </c>
       <c r="O417" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P417" s="37" t="s">
         <v>52</v>
       </c>
       <c r="Q417" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R417" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S417" s="34">
         <v>2</v>
@@ -25992,13 +26007,13 @@
         <v>3</v>
       </c>
       <c r="O418" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P418" s="37" t="s">
         <v>51</v>
       </c>
       <c r="Q418" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R418" s="22" t="s">
         <v>53</v>
@@ -26063,7 +26078,7 @@
         <v>2.5</v>
       </c>
       <c r="O419" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P419" s="37" t="s">
         <v>51</v>
@@ -26134,7 +26149,7 @@
         <v>2.7</v>
       </c>
       <c r="O420" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P420" s="37" t="s">
         <v>52</v>
@@ -26143,7 +26158,7 @@
         <v>54</v>
       </c>
       <c r="R420" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S420" s="34">
         <v>3</v>
@@ -26205,7 +26220,7 @@
         <v>2.9</v>
       </c>
       <c r="O421" s="37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P421" s="37" t="s">
         <v>52</v>
@@ -26214,7 +26229,7 @@
         <v>54</v>
       </c>
       <c r="R421" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S421" s="34">
         <v>1</v>
@@ -26276,7 +26291,7 @@
         <v>3</v>
       </c>
       <c r="O422" s="37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P422" s="37" t="s">
         <v>64</v>
@@ -26347,16 +26362,16 @@
         <v>3.6</v>
       </c>
       <c r="O423" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P423" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Q423" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R423" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S423" s="34">
         <v>2</v>
@@ -26418,7 +26433,7 @@
         <v>2.8</v>
       </c>
       <c r="O424" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P424" s="37" t="s">
         <v>52</v>
@@ -26427,7 +26442,7 @@
         <v>54</v>
       </c>
       <c r="R424" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S424" s="34">
         <v>2</v>
@@ -26471,7 +26486,7 @@
     </row>
     <row r="426" spans="1:23">
       <c r="A426" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B426" s="12"/>
       <c r="C426" s="12"/>
@@ -26690,7 +26705,7 @@
         <v>54</v>
       </c>
       <c r="R429" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S429" s="34">
         <v>3</v>
@@ -26757,11 +26772,11 @@
       <c r="P430" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Q430" s="22" t="s">
-        <v>58</v>
+      <c r="Q430" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="R430" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S430" s="34">
         <v>2</v>
@@ -26888,7 +26903,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="M432" s="34">
-        <v>1.47</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="N432" s="35">
         <v>2.8</v>
@@ -26970,8 +26985,8 @@
       <c r="P433" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Q433" s="22" t="s">
-        <v>58</v>
+      <c r="Q433" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="R433" s="22" t="s">
         <v>53</v>
@@ -27116,7 +27131,7 @@
         <v>54</v>
       </c>
       <c r="R435" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S435" s="34">
         <v>2</v>
@@ -27207,7 +27222,7 @@
     </row>
     <row r="438" spans="1:23" ht="15.75">
       <c r="A438" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B438" s="2"/>
       <c r="C438" s="2"/>
@@ -27252,10 +27267,10 @@
       <c r="L439" s="13"/>
       <c r="M439" s="12"/>
       <c r="N439" s="14"/>
-      <c r="O439" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P439" s="49"/>
+      <c r="O439" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P439" s="48"/>
       <c r="Q439" s="15"/>
       <c r="R439" s="11"/>
       <c r="S439" s="16"/>
@@ -27276,11 +27291,11 @@
       </c>
       <c r="I440" s="11"/>
       <c r="J440" s="18"/>
-      <c r="K440" s="48" t="s">
+      <c r="K440" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L440" s="48"/>
-      <c r="M440" s="48"/>
+      <c r="L440" s="49"/>
+      <c r="M440" s="49"/>
       <c r="N440" s="20" t="s">
         <v>5</v>
       </c>
@@ -27437,7 +27452,7 @@
     </row>
     <row r="443" spans="1:23">
       <c r="A443" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B443" s="29"/>
       <c r="C443" s="29"/>
@@ -27552,7 +27567,7 @@
         <v>4</v>
       </c>
       <c r="G445" s="22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H445" s="22">
         <v>3.7</v>
@@ -28197,7 +28212,7 @@
     </row>
     <row r="455" spans="1:23">
       <c r="A455" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B455" s="12"/>
       <c r="C455" s="12"/>
@@ -28330,7 +28345,7 @@
         <v>19.3</v>
       </c>
       <c r="M457" s="34">
-        <v>25.9</v>
+        <v>2.9</v>
       </c>
       <c r="N457" s="35">
         <v>2.8</v>
@@ -28383,7 +28398,7 @@
         <v>0</v>
       </c>
       <c r="G458" s="22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H458" s="22">
         <v>2.5</v>
@@ -28401,7 +28416,7 @@
         <v>17.8</v>
       </c>
       <c r="M458" s="34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N458" s="35">
         <v>2.9</v>
@@ -28487,13 +28502,13 @@
         <v>54</v>
       </c>
       <c r="R459" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S459" s="34">
         <v>2</v>
       </c>
       <c r="T459" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U459" s="34">
         <v>29</v>
@@ -28596,7 +28611,7 @@
         <v>1</v>
       </c>
       <c r="G461" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H461" s="22">
         <v>3.1</v>
@@ -28614,7 +28629,7 @@
         <v>14.5</v>
       </c>
       <c r="M461" s="34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N461" s="35">
         <v>2.8</v>
@@ -28809,7 +28824,7 @@
         <v>1</v>
       </c>
       <c r="G464" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H464" s="22">
         <v>1.5</v>
@@ -28827,7 +28842,7 @@
         <v>17.5</v>
       </c>
       <c r="M464" s="34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N464" s="35">
         <v>2.2999999999999998</v>
@@ -28933,7 +28948,7 @@
     </row>
     <row r="467" spans="1:23" ht="15.75">
       <c r="A467" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B467" s="2"/>
       <c r="C467" s="2"/>
@@ -28978,10 +28993,10 @@
       <c r="L468" s="13"/>
       <c r="M468" s="12"/>
       <c r="N468" s="14"/>
-      <c r="O468" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P468" s="49"/>
+      <c r="O468" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P468" s="48"/>
       <c r="Q468" s="15"/>
       <c r="R468" s="11"/>
       <c r="S468" s="16"/>
@@ -29002,11 +29017,11 @@
       </c>
       <c r="I469" s="11"/>
       <c r="J469" s="18"/>
-      <c r="K469" s="48" t="s">
+      <c r="K469" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L469" s="48"/>
-      <c r="M469" s="48"/>
+      <c r="L469" s="49"/>
+      <c r="M469" s="49"/>
       <c r="N469" s="20" t="s">
         <v>5</v>
       </c>
@@ -29163,7 +29178,7 @@
     </row>
     <row r="472" spans="1:23">
       <c r="A472" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B472" s="29"/>
       <c r="C472" s="29"/>
@@ -29240,13 +29255,13 @@
         <v>53</v>
       </c>
       <c r="R473" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S473" s="34">
         <v>2</v>
       </c>
       <c r="T473" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U473" s="34">
         <v>20</v>
@@ -29349,7 +29364,7 @@
         <v>2</v>
       </c>
       <c r="G475" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H475" s="22">
         <v>3.4</v>
@@ -29491,7 +29506,7 @@
         <v>0</v>
       </c>
       <c r="G477" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H477" s="22">
         <v>1.9</v>
@@ -29509,7 +29524,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="M477" s="34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N477" s="35">
         <v>3</v>
@@ -29524,7 +29539,7 @@
         <v>53</v>
       </c>
       <c r="R477" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S477" s="34">
         <v>2</v>
@@ -29580,7 +29595,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="M478" s="34">
-        <v>2.0289999999999999</v>
+        <v>3.0289999999999999</v>
       </c>
       <c r="N478" s="35">
         <v>3.1</v>
@@ -29601,7 +29616,7 @@
         <v>1</v>
       </c>
       <c r="T478" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U478" s="34">
         <v>15</v>
@@ -29672,7 +29687,7 @@
         <v>2</v>
       </c>
       <c r="T479" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U479" s="34">
         <v>21</v>
@@ -29743,7 +29758,7 @@
         <v>2</v>
       </c>
       <c r="T480" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U480" s="34">
         <v>18</v>
@@ -29775,7 +29790,7 @@
         <v>2</v>
       </c>
       <c r="G481" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H481" s="22">
         <v>2.1</v>
@@ -29793,7 +29808,7 @@
         <v>14.3</v>
       </c>
       <c r="M481" s="34" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="N481" s="35">
         <v>3</v>
@@ -29923,7 +29938,7 @@
     </row>
     <row r="484" spans="1:23">
       <c r="A484" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B484" s="12"/>
       <c r="C484" s="12"/>
@@ -30094,19 +30109,19 @@
         <v>3</v>
       </c>
       <c r="B487" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C487" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D487" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E487" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F487" s="22" t="s">
         <v>194</v>
-      </c>
-      <c r="C487" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D487" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="E487" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="F487" s="22" t="s">
-        <v>196</v>
       </c>
       <c r="G487" s="22">
         <v>3.3479999999999999</v>
@@ -30284,13 +30299,13 @@
         <v>54</v>
       </c>
       <c r="R489" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S489" s="34">
         <v>3</v>
       </c>
       <c r="T489" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U489" s="34">
         <v>17</v>
@@ -30355,13 +30370,13 @@
         <v>53</v>
       </c>
       <c r="R490" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S490" s="34">
         <v>2</v>
       </c>
       <c r="T490" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U490" s="34">
         <v>21</v>
@@ -30659,7 +30674,7 @@
     </row>
     <row r="496" spans="1:23" ht="15.75">
       <c r="A496" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B496" s="2"/>
       <c r="C496" s="2"/>
@@ -30704,10 +30719,10 @@
       <c r="L497" s="13"/>
       <c r="M497" s="12"/>
       <c r="N497" s="14"/>
-      <c r="O497" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P497" s="49"/>
+      <c r="O497" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P497" s="48"/>
       <c r="Q497" s="15"/>
       <c r="R497" s="11"/>
       <c r="S497" s="16"/>
@@ -30728,11 +30743,11 @@
       </c>
       <c r="I498" s="11"/>
       <c r="J498" s="18"/>
-      <c r="K498" s="48" t="s">
+      <c r="K498" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L498" s="48"/>
-      <c r="M498" s="48"/>
+      <c r="L498" s="49"/>
+      <c r="M498" s="49"/>
       <c r="N498" s="20" t="s">
         <v>5</v>
       </c>
@@ -30889,7 +30904,7 @@
     </row>
     <row r="501" spans="1:23">
       <c r="A501" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B501" s="29"/>
       <c r="C501" s="29"/>
@@ -31648,7 +31663,7 @@
     </row>
     <row r="513" spans="1:23">
       <c r="A513" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B513" s="12"/>
       <c r="C513" s="12"/>
@@ -32367,7 +32382,7 @@
     </row>
     <row r="525" spans="1:23" ht="15.75">
       <c r="A525" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B525" s="2"/>
       <c r="C525" s="2"/>
@@ -32412,10 +32427,10 @@
       <c r="L526" s="13"/>
       <c r="M526" s="12"/>
       <c r="N526" s="14"/>
-      <c r="O526" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P526" s="49"/>
+      <c r="O526" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P526" s="48"/>
       <c r="Q526" s="15"/>
       <c r="R526" s="11"/>
       <c r="S526" s="16"/>
@@ -32436,11 +32451,11 @@
       </c>
       <c r="I527" s="11"/>
       <c r="J527" s="18"/>
-      <c r="K527" s="48" t="s">
+      <c r="K527" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L527" s="48"/>
-      <c r="M527" s="48"/>
+      <c r="L527" s="49"/>
+      <c r="M527" s="49"/>
       <c r="N527" s="20" t="s">
         <v>5</v>
       </c>
@@ -32597,7 +32612,7 @@
     </row>
     <row r="530" spans="1:23">
       <c r="A530" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B530" s="29"/>
       <c r="C530" s="29"/>
@@ -32650,7 +32665,7 @@
         <v>0</v>
       </c>
       <c r="J531" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K531" s="34">
         <v>16</v>
@@ -32674,7 +32689,7 @@
         <v>53</v>
       </c>
       <c r="R531" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S531" s="34">
         <v>2</v>
@@ -32928,7 +32943,7 @@
         <v>2.8660000000000001</v>
       </c>
       <c r="H535" s="22">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="I535" s="22">
         <v>0</v>
@@ -32996,7 +33011,7 @@
         <v>2</v>
       </c>
       <c r="G536" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H536" s="22">
         <v>2.2999999999999998</v>
@@ -33041,7 +33056,7 @@
         <v>10</v>
       </c>
       <c r="V536" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W536">
         <v>2</v>
@@ -33280,7 +33295,7 @@
         <v>0</v>
       </c>
       <c r="G540" s="22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H540" s="22">
         <v>3.2</v>
@@ -33357,7 +33372,7 @@
     </row>
     <row r="542" spans="1:23">
       <c r="A542" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B542" s="12"/>
       <c r="C542" s="12"/>
@@ -33434,13 +33449,13 @@
         <v>53</v>
       </c>
       <c r="R543" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S543" s="34">
         <v>1</v>
       </c>
       <c r="T543" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U543" s="34">
         <v>5</v>
@@ -33505,13 +33520,13 @@
         <v>54</v>
       </c>
       <c r="R544" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S544" s="34">
         <v>2</v>
       </c>
       <c r="T544" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U544" s="34">
         <v>27</v>
@@ -33898,7 +33913,7 @@
         <v>0</v>
       </c>
       <c r="G550" s="22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H550" s="22">
         <v>5</v>
@@ -34043,7 +34058,7 @@
         <v>3.1960000000000002</v>
       </c>
       <c r="H552" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I552" s="22">
         <v>0</v>
@@ -34138,10 +34153,10 @@
       <c r="L555" s="13"/>
       <c r="M555" s="12"/>
       <c r="N555" s="14"/>
-      <c r="O555" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P555" s="49"/>
+      <c r="O555" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P555" s="48"/>
       <c r="Q555" s="15"/>
       <c r="R555" s="11"/>
       <c r="S555" s="16"/>
@@ -34162,11 +34177,11 @@
       </c>
       <c r="I556" s="11"/>
       <c r="J556" s="18"/>
-      <c r="K556" s="48" t="s">
+      <c r="K556" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L556" s="48"/>
-      <c r="M556" s="48"/>
+      <c r="L556" s="49"/>
+      <c r="M556" s="49"/>
       <c r="N556" s="20" t="s">
         <v>5</v>
       </c>
@@ -34323,7 +34338,7 @@
     </row>
     <row r="559" spans="1:23">
       <c r="A559" s="28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C559" s="29"/>
       <c r="D559" s="29"/>
@@ -34902,7 +34917,7 @@
         <v>2</v>
       </c>
       <c r="T567" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U567" s="34">
         <v>17</v>
@@ -35082,7 +35097,7 @@
     </row>
     <row r="571" spans="1:23">
       <c r="A571" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B571" s="12"/>
       <c r="C571" s="12"/>
@@ -35197,7 +35212,7 @@
         <v>1</v>
       </c>
       <c r="G573" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H573" s="22">
         <v>3.9</v>
@@ -35339,7 +35354,7 @@
         <v>0</v>
       </c>
       <c r="G575" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H575" s="22">
         <v>3.5</v>
@@ -35552,7 +35567,7 @@
         <v>0</v>
       </c>
       <c r="G578" s="22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H578" s="22">
         <v>4.3</v>
@@ -35623,7 +35638,7 @@
         <v>2</v>
       </c>
       <c r="G579" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H579" s="22">
         <v>2.2000000000000002</v>
@@ -35641,7 +35656,7 @@
         <v>16.5</v>
       </c>
       <c r="M579" s="34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N579" s="35">
         <v>3</v>
@@ -35818,66 +35833,66 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="O91:P91"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="Q92:R92"/>
+    <mergeCell ref="O120:P120"/>
+    <mergeCell ref="K121:M121"/>
+    <mergeCell ref="Q121:R121"/>
+    <mergeCell ref="O149:P149"/>
+    <mergeCell ref="K150:M150"/>
+    <mergeCell ref="Q150:R150"/>
+    <mergeCell ref="O178:P178"/>
+    <mergeCell ref="K179:M179"/>
+    <mergeCell ref="Q179:R179"/>
+    <mergeCell ref="O207:P207"/>
+    <mergeCell ref="K208:M208"/>
+    <mergeCell ref="Q208:R208"/>
+    <mergeCell ref="O236:P236"/>
+    <mergeCell ref="K237:M237"/>
+    <mergeCell ref="Q237:R237"/>
+    <mergeCell ref="O265:P265"/>
+    <mergeCell ref="K266:M266"/>
+    <mergeCell ref="Q266:R266"/>
+    <mergeCell ref="O294:P294"/>
+    <mergeCell ref="K295:M295"/>
+    <mergeCell ref="Q295:R295"/>
+    <mergeCell ref="O323:P323"/>
+    <mergeCell ref="K324:M324"/>
+    <mergeCell ref="Q324:R324"/>
+    <mergeCell ref="O352:P352"/>
+    <mergeCell ref="K353:M353"/>
+    <mergeCell ref="Q353:R353"/>
+    <mergeCell ref="O381:P381"/>
+    <mergeCell ref="K382:M382"/>
+    <mergeCell ref="Q382:R382"/>
+    <mergeCell ref="O410:P410"/>
+    <mergeCell ref="K411:M411"/>
+    <mergeCell ref="Q411:R411"/>
+    <mergeCell ref="O439:P439"/>
+    <mergeCell ref="K440:M440"/>
+    <mergeCell ref="Q440:R440"/>
+    <mergeCell ref="O468:P468"/>
+    <mergeCell ref="K469:M469"/>
+    <mergeCell ref="Q469:R469"/>
+    <mergeCell ref="O497:P497"/>
+    <mergeCell ref="K498:M498"/>
+    <mergeCell ref="Q498:R498"/>
     <mergeCell ref="O526:P526"/>
     <mergeCell ref="K527:M527"/>
     <mergeCell ref="Q527:R527"/>
     <mergeCell ref="O555:P555"/>
     <mergeCell ref="K556:M556"/>
     <mergeCell ref="Q556:R556"/>
-    <mergeCell ref="O468:P468"/>
-    <mergeCell ref="K469:M469"/>
-    <mergeCell ref="Q469:R469"/>
-    <mergeCell ref="O497:P497"/>
-    <mergeCell ref="K498:M498"/>
-    <mergeCell ref="Q498:R498"/>
-    <mergeCell ref="O410:P410"/>
-    <mergeCell ref="K411:M411"/>
-    <mergeCell ref="Q411:R411"/>
-    <mergeCell ref="O439:P439"/>
-    <mergeCell ref="K440:M440"/>
-    <mergeCell ref="Q440:R440"/>
-    <mergeCell ref="O352:P352"/>
-    <mergeCell ref="K353:M353"/>
-    <mergeCell ref="Q353:R353"/>
-    <mergeCell ref="O381:P381"/>
-    <mergeCell ref="K382:M382"/>
-    <mergeCell ref="Q382:R382"/>
-    <mergeCell ref="O294:P294"/>
-    <mergeCell ref="K295:M295"/>
-    <mergeCell ref="Q295:R295"/>
-    <mergeCell ref="O323:P323"/>
-    <mergeCell ref="K324:M324"/>
-    <mergeCell ref="Q324:R324"/>
-    <mergeCell ref="O236:P236"/>
-    <mergeCell ref="K237:M237"/>
-    <mergeCell ref="Q237:R237"/>
-    <mergeCell ref="O265:P265"/>
-    <mergeCell ref="K266:M266"/>
-    <mergeCell ref="Q266:R266"/>
-    <mergeCell ref="O178:P178"/>
-    <mergeCell ref="K179:M179"/>
-    <mergeCell ref="Q179:R179"/>
-    <mergeCell ref="O207:P207"/>
-    <mergeCell ref="K208:M208"/>
-    <mergeCell ref="Q208:R208"/>
-    <mergeCell ref="O120:P120"/>
-    <mergeCell ref="K121:M121"/>
-    <mergeCell ref="Q121:R121"/>
-    <mergeCell ref="O149:P149"/>
-    <mergeCell ref="K150:M150"/>
-    <mergeCell ref="Q150:R150"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="O91:P91"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="Q92:R92"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="Q34:R34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>